<commit_message>
adds Multiplayer and competitors, as well as a help section with interactive guides and a documentation
</commit_message>
<xml_diff>
--- a/finanzen.xlsx
+++ b/finanzen.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Startkapital" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Kredite" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sonstiges" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Transportkosten" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -468,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +545,22 @@
       </c>
       <c r="D4" t="n">
         <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sofortkredit</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -630,4 +647,93 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Transportart</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Kosten_pro_km</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Basis_Transportkosten</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Mindestkosten</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Standard Lieferung</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Express Lieferung</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sperrgut</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>